<commit_message>
Table name protection from "too long"
</commit_message>
<xml_diff>
--- a/src/persistence/Persistence.Tests/Assets/OpinionFile.xlsx
+++ b/src/persistence/Persistence.Tests/Assets/OpinionFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CF481C-C484-4E2C-BC46-75434A7BE19F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B568AC-EFF4-4290-BEDD-5CFFFBE48853}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Answer*</t>
+  </si>
+  <si>
+    <t>Space Column</t>
   </si>
 </sst>
 </file>
@@ -402,11 +405,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D512E07-522C-4FA9-9571-8CE2D6A4A9EC}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -415,7 +416,7 @@
     <col min="4" max="4" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -428,8 +429,11 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -443,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -457,7 +461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -471,7 +475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -485,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>